<commit_message>
adding a few figures
</commit_message>
<xml_diff>
--- a/parameters/Task13_Param_Ranges_AFIR_Tfold.xlsx
+++ b/parameters/Task13_Param_Ranges_AFIR_Tfold.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/git/TMDD_EndogenousLigand/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6EC7C9-5A26-FD4B-BDF3-76D8A1C93870}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053B7006-1EC5-A745-9993-3977C86993D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40840" yWindow="1200" windowWidth="27300" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="27300" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task05_Param_Summary" sheetId="1" r:id="rId1"/>
@@ -245,7 +245,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,6 +395,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF0432FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF0432FF"/>
       <name val="Calibri"/>
@@ -743,7 +759,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -775,7 +791,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -784,6 +800,19 @@
     <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1274,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="163" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="163" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1897,27 +1926,27 @@
       <c r="C18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="18">
         <f>D19/E20</f>
         <v>7</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="18">
         <f>E19/D20</f>
         <v>40320</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="19">
         <v>0.1</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="19">
         <v>10</v>
       </c>
-      <c r="I18" s="14">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="I18" s="19">
+        <v>0</v>
+      </c>
+      <c r="J18" s="20" t="s">
         <v>46</v>
       </c>
       <c r="K18" s="1" t="s">
@@ -1969,29 +1998,29 @@
       <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="16">
         <f>1/28</f>
         <v>3.5714285714285712E-2</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="16">
         <f>1/7</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="F20" s="11">
-        <v>0</v>
-      </c>
-      <c r="G20" s="14">
+      <c r="F20" s="17">
+        <v>0</v>
+      </c>
+      <c r="G20" s="19">
         <f>G19/H18</f>
         <v>0.1</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="19">
         <f>H19/G18</f>
         <v>14400</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="20" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2113,15 +2142,15 @@
       <c r="C24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <f>D23/E22</f>
         <v>0.1</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="9">
         <f>E23/D22</f>
         <v>14400</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="13" t="s">
         <v>50</v>
       </c>
       <c r="G24" s="12">

</xml_diff>